<commit_message>
Fix test data for cubic spline
</commit_message>
<xml_diff>
--- a/test/Tests.xlsx
+++ b/test/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -461,7 +461,7 @@
       </c>
       <c r="B4">
         <f>Interpolation!F1</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <f>Interpolation!F2</f>
@@ -474,7 +474,7 @@
       </c>
       <c r="B6">
         <f>SUM($B$4:B5)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <f>SUM($C$4:C5)</f>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="F1">
         <f>COUNTIF(D16:D22,"=TRUE")+COUNTIF(I16:I22,"=TRUE")</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -687,11 +687,11 @@
         <v>-4.0292960501411151E-4</v>
       </c>
       <c r="H17" s="4">
-        <v>1.74457358059E-4</v>
+        <v>-4.02929605014E-4</v>
       </c>
       <c r="I17" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -715,11 +715,11 @@
         <v>8.7690201405915547E-2</v>
       </c>
       <c r="H18" s="4">
-        <v>9.0527195350326994E-2</v>
+        <v>8.7690201405916005E-2</v>
       </c>
       <c r="I18" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>0.8414709848078965</v>
       </c>
       <c r="H19" s="4">
-        <v>0.84147098480789595</v>
+        <v>0.84147098480789695</v>
       </c>
       <c r="I19" t="b">
         <f t="shared" si="2"/>
@@ -771,7 +771,7 @@
         <v>4.579094280463962E-2</v>
       </c>
       <c r="H20" s="4">
-        <v>4.5790942804639002E-2</v>
+        <v>4.5790942804640002E-2</v>
       </c>
       <c r="I20" t="b">
         <f t="shared" si="2"/>
@@ -785,9 +785,12 @@
       <c r="B21">
         <v>1.228293256202952</v>
       </c>
+      <c r="C21">
+        <v>1.22829325620295</v>
+      </c>
       <c r="D21" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -795,9 +798,12 @@
       <c r="G21">
         <v>1.228293256202952</v>
       </c>
+      <c r="H21" s="4">
+        <v>1.22829325620295</v>
+      </c>
       <c r="I21" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,9 +813,12 @@
       <c r="B22">
         <v>4.579094202585117E-2</v>
       </c>
+      <c r="C22">
+        <v>4.5790942025851003E-2</v>
+      </c>
       <c r="D22" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
         <v>9.0000000100000008</v>
@@ -817,9 +826,12 @@
       <c r="G22">
         <v>4.5790941810737687E-2</v>
       </c>
+      <c r="H22" s="4">
+        <v>4.5790941810737999E-2</v>
+      </c>
       <c r="I22" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add linalg module with solve function
</commit_message>
<xml_diff>
--- a/test/Tests.xlsx
+++ b/test/Tests.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Interpolation" sheetId="2" r:id="rId2"/>
+    <sheet name="LinAlg" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>LINEAR</t>
   </si>
@@ -61,6 +62,24 @@
   </si>
   <si>
     <t>Module</t>
+  </si>
+  <si>
+    <t>Solve</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>x (solution)</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
   </si>
 </sst>
 </file>
@@ -71,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +101,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -108,12 +134,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,17 +502,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <f>LinAlg!F1</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>LinAlg!F2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <f>SUM($B$4:B5)</f>
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <f>SUM($C$4:C5)</f>
-        <v>14</v>
+      <c r="B7">
+        <f>SUM($B$4:B6)</f>
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f>SUM($C$4:C6)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -491,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,9 +563,6 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
@@ -528,82 +572,87 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B11" si="0">SIN(A3)/A3</f>
-        <v>0.8414709848078965</v>
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B12" si="0">SIN(A4)/A4</f>
+        <v>0.8414709848078965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>0.45464871341284085</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>4.7040002686622402E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>-0.18920062382698205</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>-0.1917848549326277</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>-4.6569249699820979E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>9.3855228388398437E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>0.12366978082792272</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>4.579094280463962E-2</v>
       </c>
@@ -641,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <f t="array" ref="B16:B22">_xll.NUM.INTERP.LINEAR($A$3:$A$11,$B$3:$B$11,A16:A22)</f>
+        <f t="array" ref="B16:B22">_xll.NUM.INTERP.LINEAR($A$4:$A$12,$B$4:$B$12,A16:A22)</f>
         <v>-0.18920062382698205</v>
       </c>
       <c r="C16" s="3">
@@ -655,7 +704,7 @@
         <v>4</v>
       </c>
       <c r="G16">
-        <f t="array" ref="G16:G22">_xll.NUM.INTERP.CUBIC(A3:A11,B3:B11,F16:F22)</f>
+        <f t="array" ref="G16:G22">_xll.NUM.INTERP.CUBIC(A4:A12,B4:B12,F16:F22)</f>
         <v>-0.18920062382698205</v>
       </c>
       <c r="H16" s="4">
@@ -833,6 +882,286 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1">
+        <f>COUNTIF(D13,"=TRUE")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>-4.0959561062000001E-2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-9.6797637241999995E-2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-1.8938374354E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-0.15669789463799999</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2.3600206203999999E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>9.3516508334000006E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>0.20860531099999999</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5.2551509575000002E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.27287816833099998</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9.2840307449000001E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.35674078743900001</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-0.23932867955600001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>0.19802329771999999</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-0.13349903071499999</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.29416969299700002</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-0.25298770034700002</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-5.7024024830999998E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-0.31116030492699998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>-0.26431565513100003</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.13869637729100001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-0.31843275477600003</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-0.41361038225699998</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-0.31357978875499998</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.24258915628800001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>0.13429144351799999</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.14247961538500001</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.27478575220599999</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.17916673615600001</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.396729642652</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.19738717125300001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>0.18991817161999999</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-3.2597967584999998E-2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-6.7951351884999997E-2</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.23654768926799999</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-4.5720609618000001E-2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.16478260505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>0.83749499000000005</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="array" ref="B13:B18">_xll.NUM.LINALG.SOLVE(A6:F11,A13:A18)</f>
+        <v>2.7508954943328487</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2.7508954943328399</v>
+      </c>
+      <c r="D13" s="8" t="b">
+        <f>MAX(ABS(B13:B18-C13:C18))&lt;B1</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>0.13441411</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-1.6153695061082334</v>
+      </c>
+      <c r="C14" s="7">
+        <v>-1.61536950610823</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>0.52464785000000003</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.31235615273604794</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.312356152736048</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>0.42286944999999998</v>
+      </c>
+      <c r="B16" s="5">
+        <v>-2.967064411098828</v>
+      </c>
+      <c r="C16" s="7">
+        <v>-2.96706441109882</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>0.97604661999999998</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1.6600662213689663</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1.6600662213689601</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>0.29701416000000003</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3.1610608855991846</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3.1610608855991802</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add union type for excel success/error
With downcasting to obj for compatibility with ExcelDNA
</commit_message>
<xml_diff>
--- a/test/Tests.xlsx
+++ b/test/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>